<commit_message>
First version of module for release
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_1.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magzumov\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magzumov\IdeaProjects\unic\nicnbk-data\nicnbk-data-service-impl\src\main\resources\export_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Database">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ОФП_1!$A$1:$F$81</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateCount="10000" iterateDelta="1E-10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>Код формы</t>
   </si>
@@ -1311,6 +1311,18 @@
   </si>
   <si>
     <t>по состоянию на дату</t>
+  </si>
+  <si>
+    <t>&lt;dd.MM.yyyy&gt;</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
   </si>
 </sst>
 </file>
@@ -1320,9 +1332,9 @@
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.0000\ _₽_-;\-* #,##0.0000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0000\ _₽_-;\-* #,##0.0000\ _₽_-;_-* &quot;-&quot;????????\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00000\ _₽_-;\-* #,##0.00000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0000\ _₽_-;\-* #,##0.0000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0000\ _₽_-;\-* #,##0.0000\ _₽_-;_-* &quot;-&quot;????????\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00000\ _₽_-;\-* #,##0.00000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1423,18 +1435,12 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -1519,8 +1525,8 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1533,7 +1539,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1555,7 +1561,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1590,6 +1596,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1597,7 +1604,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1921,8 +1927,8 @@
   </sheetPr>
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:F10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2712,8 +2718,8 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="49">
-        <v>42979</v>
+      <c r="C2" s="46" t="s">
+        <v>126</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>4</v>
@@ -2747,24 +2753,24 @@
       <c r="F7" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -2993,8 +2999,8 @@
       <c r="B28" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="21">
-        <v>14</v>
+      <c r="C28" s="13" t="s">
+        <v>127</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="43"/>
@@ -3162,8 +3168,8 @@
       <c r="B40" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="25">
-        <v>26</v>
+      <c r="C40" s="13" t="s">
+        <v>128</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="43"/>
@@ -3178,8 +3184,8 @@
       <c r="B41" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C41" s="21">
-        <v>27</v>
+      <c r="C41" s="13" t="s">
+        <v>129</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="43"/>
@@ -3527,24 +3533,24 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="26"/>
-      <c r="B68" s="47" t="s">
+      <c r="B68" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="C68" s="48"/>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="48"/>
+      <c r="C68" s="49"/>
+      <c r="D68" s="49"/>
+      <c r="E68" s="49"/>
+      <c r="F68" s="49"/>
       <c r="G68" s="19"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="26"/>
-      <c r="B69" s="47" t="s">
+      <c r="B69" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="C69" s="48"/>
-      <c r="D69" s="48"/>
-      <c r="E69" s="48"/>
-      <c r="F69" s="48"/>
+      <c r="C69" s="49"/>
+      <c r="D69" s="49"/>
+      <c r="E69" s="49"/>
+      <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="26"/>

</xml_diff>

<commit_message>
Fix NBRK reporting module: - export EXCEL templates font (bold/not bold) - export temp files cleaning - GL Tarragon form editing added records - GL Tarragon form - drop down list of funds for "Net Realized .." added records 0 etc
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_1.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_1.xlsx
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Database">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ОФП_1!$A$1:$F$81</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateCount="10000" iterateDelta="1E-10"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1487,7 +1487,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1597,6 +1597,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1604,6 +1605,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1927,8 +1929,8 @@
   </sheetPr>
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65:F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2753,24 +2755,24 @@
       <c r="F7" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -2821,8 +2823,8 @@
         <v>16</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
     </row>
@@ -2989,8 +2991,8 @@
         <v>40</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
       <c r="G27" s="14"/>
       <c r="H27" s="18"/>
     </row>
@@ -3003,8 +3005,8 @@
         <v>127</v>
       </c>
       <c r="D28" s="12"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
       <c r="G28" s="22"/>
       <c r="H28" s="18"/>
     </row>
@@ -3158,8 +3160,8 @@
         <v>63</v>
       </c>
       <c r="D39" s="13"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
       <c r="G39" s="22"/>
       <c r="H39" s="18"/>
     </row>
@@ -3172,8 +3174,8 @@
         <v>128</v>
       </c>
       <c r="D40" s="25"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
       <c r="G40" s="22"/>
       <c r="H40" s="18"/>
       <c r="I40" s="23"/>
@@ -3188,8 +3190,8 @@
         <v>129</v>
       </c>
       <c r="D41" s="12"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
       <c r="G41" s="14"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -3292,8 +3294,8 @@
         <v>81</v>
       </c>
       <c r="D49" s="13"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="51"/>
       <c r="G49" s="14"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3305,8 +3307,8 @@
         <v>83</v>
       </c>
       <c r="D50" s="17"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
       <c r="G50" s="19"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3396,8 +3398,8 @@
         <v>97</v>
       </c>
       <c r="D57" s="13"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
       <c r="G57" s="19"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3409,8 +3411,8 @@
         <v>44</v>
       </c>
       <c r="D58" s="12"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
       <c r="G58" s="19"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3502,8 +3504,8 @@
         <v>111</v>
       </c>
       <c r="D65" s="13"/>
-      <c r="E65" s="43"/>
-      <c r="F65" s="43"/>
+      <c r="E65" s="47"/>
+      <c r="F65" s="47"/>
       <c r="G65" s="19"/>
       <c r="H65" s="18"/>
       <c r="I65" s="23"/>
@@ -3517,8 +3519,8 @@
         <v>113</v>
       </c>
       <c r="D66" s="13"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
       <c r="G66" s="19"/>
       <c r="I66" s="19"/>
       <c r="J66" s="19"/>
@@ -3533,24 +3535,24 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="26"/>
-      <c r="B68" s="48" t="s">
+      <c r="B68" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="C68" s="49"/>
-      <c r="D68" s="49"/>
-      <c r="E68" s="49"/>
-      <c r="F68" s="49"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="50"/>
       <c r="G68" s="19"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="26"/>
-      <c r="B69" s="48" t="s">
+      <c r="B69" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="C69" s="49"/>
-      <c r="D69" s="49"/>
-      <c r="E69" s="49"/>
-      <c r="F69" s="49"/>
+      <c r="C69" s="50"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="50"/>
+      <c r="F69" s="50"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="26"/>

</xml_diff>

<commit_message>
NB Reporting Module: - changes according to NB forms update (IFRS 9) - form 7 and form 1 done
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_1.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_1.xlsx
@@ -18,9 +18,9 @@
     <definedName name="GR_CODE_ROW">4583</definedName>
     <definedName name="GR_CODE_SHEET">4</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ОФП_1!$A$1:$F$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ОФП_1!$A$1:$F$83</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>Код формы</t>
   </si>
@@ -101,913 +101,99 @@
     <t>2</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Вклады размещенные (за вычетом резервов на обесценение) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">(1150.020-1150.100, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>1160.070,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>1160.080,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">1270.090-1270.110, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>1290.070,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>1290.090</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Финансовые инвестиции, оцениваемые по справедливой стоимости, изменения которой отражаются в составе прибыли или убытка </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(1120, 1270.020, 1270.050)</t>
-    </r>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Финансовые инвестиции, имеющиеся в наличии для продажи (за вычетом резервов на обесценение) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">(1140, 1160.050, 1160.060, 1270.040, 1270.070, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>1290.050</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Финансовые инвестиции, удерживаемые до погашения (за вычетом резервов на обесценение) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">(1130, 1160.030, 1160.040, 1270.030, 1270.060, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>1290.030</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Прочие краткосрочные финансовые инвестиции </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(1110, 1150.010, 1150.110-1150.140, 1160.010, 1160.020, 1160.090, 1270.010, 1270.080, 1270.120, 1270.130, 1280.010, 1290.010, 1290.110, 1290.130)</t>
-    </r>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Краткосрочная торговая и прочая дебиторская задолженность </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>1210-1260, 1280.020, 1290.130, 1610</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Текущие налоговые активы </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(1410-1430)</t>
-    </r>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Запасы </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(1310-1360)</t>
-    </r>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Прочие краткосрочные активы </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>1620</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>, 1630)</t>
-    </r>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Активы (или выбывающие группы), предназначенные для продажи </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(1510-1520)</t>
-    </r>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
-    <t>Итого краткосрочных активов (сумма строк 2-12)</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
     <t>Долгосрочные активы</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Вклады размещенные (за вычетом резервов на обесценение) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">2040.010-2040.060, 2050.070, 2050.080, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">2170.060, 2170.070, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>1290.080, 1290.100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Финансовые инвестиции, имеющиеся в наличии для продажи (за вычетом резервов на обесценение) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">(2030, 2050.050, 2050.060, 2170.030, 2170,050, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>1290.060</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Финансовые инвестиции, удерживаемые до погашения (за вычетом резервов на обесценение) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">(2020, 2050.030, 2050.040, 2170.020, 2170.040, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>1290.040</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Прочие долгосрочные финансовые инвестиции </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">(2010, 2040.070-2040.100, 2050.010, 2050.020, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>2170.010, 2170.080, 1290.020, 1290.120, 1290.130</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Долгосрочная торговая и прочая дебиторская задолженность </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>2110-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>2160, 2180, 2910</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Инвестиции, учитываемые методом долевого участия </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(2210)</t>
-    </r>
-  </si>
-  <si>
     <t>20</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Основные средства </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(2410-2430)</t>
-    </r>
-  </si>
-  <si>
     <t>21</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Нематериальные активы </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(2730</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>-2750)</t>
-    </r>
-  </si>
-  <si>
     <t>22</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Отложенные налоговые активы </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(2810)</t>
-    </r>
-  </si>
-  <si>
     <t>23</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Прочие долгосрочные активы </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>2310-2330, 2510-2520, 2610-2630, 2920-2940</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>24</t>
   </si>
   <si>
-    <t>Итого долгосрочных активов (сумма строк 15-24)</t>
-  </si>
-  <si>
     <t>25</t>
   </si>
   <si>
-    <t>Всего активы (сумма строк 13, 25)</t>
-  </si>
-  <si>
     <t>Краткосрочные обязательства</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Займы полученные </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(3010, 3020, 3380.010, 3380.020)</t>
-    </r>
-  </si>
-  <si>
     <t>28</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Прочие краткосрочные финансовые обязательства </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>3040</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>, 3050, 3380.030-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>3380.050,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> 3390.010)</t>
-    </r>
-  </si>
-  <si>
     <t>29</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Краткосрочная торговая и прочая кредиторская задолженность </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>3310-3340, 3360, 3390.020, 3510</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Краткосрочные резервы </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(3410-3440)</t>
-    </r>
-  </si>
-  <si>
     <t>31</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Текущие налоговые обязательства </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">(3110-3190, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>3210-3240)</t>
-    </r>
-  </si>
-  <si>
     <t>32</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Прочие краткосрочные обязательства </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">(3030, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>3350, 3370</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>, 3520, 3540)</t>
-    </r>
-  </si>
-  <si>
     <t>33</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Обязательства выбывающих групп, предназначенных для продажи </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(3530)</t>
-    </r>
-  </si>
-  <si>
     <t>34</t>
   </si>
   <si>
-    <t>Итого краткосрочных обязательств (сумма строк 28-34)</t>
-  </si>
-  <si>
     <t>35</t>
   </si>
   <si>
@@ -1017,263 +203,51 @@
     <t>36</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Займы полученные </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(4010, 4020, 4160.010, 4160.020)</t>
-    </r>
-  </si>
-  <si>
     <t>37</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Прочие долгосрочные финансовые обязательства </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(4030, 4160.030-4160.040)</t>
-    </r>
-  </si>
-  <si>
     <t>38</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Долгосрочная торговая и прочая кредиторская задолженность </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">(4110-4150, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>4170, 4410</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>39</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Долгосрочные резервы </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(4210-4240)</t>
-    </r>
-  </si>
-  <si>
     <t>40</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Отложенные налоговые обязательства </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(4310)</t>
-    </r>
-  </si>
-  <si>
     <t>41</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Прочие долгосрочные обязательства </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(4420, 4430)</t>
-    </r>
-  </si>
-  <si>
     <t>42</t>
   </si>
   <si>
-    <t>Итого долгосрочных обязательств (сумма строк 37-42)</t>
-  </si>
-  <si>
     <t>43</t>
   </si>
   <si>
     <t>Капитал</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Уставный капитал </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(5010-5030)</t>
-    </r>
-  </si>
-  <si>
     <t>45</t>
   </si>
   <si>
     <t>46</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Выкупленные собственные долевые инструменты </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(5210)</t>
-    </r>
-  </si>
-  <si>
     <t>47</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Резервный капитал </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">(5410, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>5460</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>48</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Прочие резервы </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(5420-5450)</t>
-    </r>
-  </si>
-  <si>
     <t>49</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Нераспределенная прибыль (непокрытый убыток) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(5510, 5520)</t>
-    </r>
-  </si>
-  <si>
     <t>50</t>
   </si>
   <si>
-    <t>Итого капитал (сумма строк 45-50)</t>
-  </si>
-  <si>
     <t>51</t>
   </si>
   <si>
-    <t>Всего обязательства и капитал (сумма строк 35, 43, 51)</t>
-  </si>
-  <si>
     <t>52</t>
   </si>
   <si>
@@ -1304,9 +278,6 @@
     <t>Наименование организации: NICK Master Fund Ltd.</t>
   </si>
   <si>
-    <t>Дополнительно оплаченный капитал (5310)</t>
-  </si>
-  <si>
     <t>Рысбеков С.Д.</t>
   </si>
   <si>
@@ -1323,6 +294,156 @@
   </si>
   <si>
     <t>27</t>
+  </si>
+  <si>
+    <t>Вклады размещенные (за вычетом резервов на обесценение) (1170, 1180.020, 1180.030, 1290.070)</t>
+  </si>
+  <si>
+    <t>Финансовые инвестиции, оцениваемые по справедливой стоимости через прибыль или убыток (1120, 1180.040, 1180.070)</t>
+  </si>
+  <si>
+    <t>Финансовые инвестиции, оцениваемые по справедливой стоимости через прочий совокупный доход (1140, 1180.050, 1180.080)</t>
+  </si>
+  <si>
+    <t>Финансовые инвестиции, оцениваемые по амортизированной стоимости (за вычетом резервов на обесценение) (1130, 1180.060, 1180.090, 1290.030)</t>
+  </si>
+  <si>
+    <t>Заемные операции (за вычетом резервов на обесценение) (1110, 1180.100, 1290.010)</t>
+  </si>
+  <si>
+    <t>Прочие краткосрочные финансовые инвестиции (1150.010, 1150.140, 1150.150, 1180.110, 1180.120, 1290.130)</t>
+  </si>
+  <si>
+    <t>Краткосрочная торговая и прочая дебиторская задолженность (1210, 1250, 1260, 1280.020, 1280.040, 1180.010, 1290.130, 1290.140)</t>
+  </si>
+  <si>
+    <t>Текущие налоговые активы (1410-1430)</t>
+  </si>
+  <si>
+    <t>Запасы (1310-1360)</t>
+  </si>
+  <si>
+    <t>Прочие краткосрочные активы (1610-1630, 1290.130)</t>
+  </si>
+  <si>
+    <t>Активы (или выбывающие группы), предназначенные для продажи (1510-1520)</t>
+  </si>
+  <si>
+    <t>Итого краткосрочных активов (сумма строк 2-13)</t>
+  </si>
+  <si>
+    <t>Вклады размещенные (за вычетом резервов на обесценение) (2060, 2070.010, 1290.080)</t>
+  </si>
+  <si>
+    <t>Финансовые инвестиции, оцениваемые по справедливой стоимости через прочий совокупный доход (2030, 2070.020, 2070.040)</t>
+  </si>
+  <si>
+    <t>Финансовые инвестиции, оцениваемые по амортизированной стоимости (за вычетом резервов на обесценение) (2020, 2070.030, 2070.050, 1290.040)</t>
+  </si>
+  <si>
+    <t>Заемные операции (за вычетом резервов на обесценение) (2010, 2070.060, 1290.020)</t>
+  </si>
+  <si>
+    <t>Прочие долгосрочные финансовые инвестиции (2040.100, 2070.070, 1290.130)</t>
+  </si>
+  <si>
+    <t>Долгосрочная торговая и прочая дебиторская задолженность (2110, 2150, 2160, 2180, 1290.150)</t>
+  </si>
+  <si>
+    <t>Инвестиции в дочерние организации, ассоциированные организации и совместные организации (2210)</t>
+  </si>
+  <si>
+    <t>Основные средства (2410-2430)</t>
+  </si>
+  <si>
+    <t>Нематериальные активы (2730-2750)</t>
+  </si>
+  <si>
+    <t>Отложенные налоговые активы (2810)</t>
+  </si>
+  <si>
+    <t>Прочие долгосрочные активы (2310-2330, 2910-2950, 1290.130)</t>
+  </si>
+  <si>
+    <t>Итого долгосрочных активов (сумма строк 16-26)</t>
+  </si>
+  <si>
+    <t>Всего активы (сумма строк 14, 27)</t>
+  </si>
+  <si>
+    <t>Займы полученные (3010, 3020, 3060.010, 3060.020)</t>
+  </si>
+  <si>
+    <t>Прочие краткосрочные финансовые обязательства (3050, 3060.030-3060.050)</t>
+  </si>
+  <si>
+    <t>Краткосрочная торговая и прочая кредиторская задолженность (3310, 3360, 3390.020, 3390.030)</t>
+  </si>
+  <si>
+    <t>Краткосрочные резервы (3410-3440)</t>
+  </si>
+  <si>
+    <t>Текущие налоговые обязательства (3110-3190, 3210-3250)</t>
+  </si>
+  <si>
+    <t>Прочие краткосрочные обязательства (3030, 3350, 3510, 3520, 3540)</t>
+  </si>
+  <si>
+    <t>Обязательства выбывающих групп, предназначенных для продажи (3530)</t>
+  </si>
+  <si>
+    <t>Итого краткосрочных обязательств (сумма строк 30-36)</t>
+  </si>
+  <si>
+    <t>Займы полученные (4010, 4020, 4040.010, 4040.020)</t>
+  </si>
+  <si>
+    <t>Прочие долгосрочные финансовые обязательства (4030, 4040.030-4040.040)</t>
+  </si>
+  <si>
+    <t>Долгосрочная торговая и прочая кредиторская задолженность (4110, 4150, 4170)</t>
+  </si>
+  <si>
+    <t>Долгосрочные резервы (4210-4240)</t>
+  </si>
+  <si>
+    <t>Отложенные налоговые обязательства (4310)</t>
+  </si>
+  <si>
+    <t>Прочие долгосрочные обязательства (4410-4430, 4180)</t>
+  </si>
+  <si>
+    <t>Итого долгосрочных обязательств (сумма строк 39-44)</t>
+  </si>
+  <si>
+    <t>Уставный капитал (5010-5030)</t>
+  </si>
+  <si>
+    <t>Дополнительно оплаченный капитал (5310, 5320)</t>
+  </si>
+  <si>
+    <t>Выкупленные собственные долевые инструменты (5210)</t>
+  </si>
+  <si>
+    <t>Резервный капитал (5410, 5460)</t>
+  </si>
+  <si>
+    <t>Прочие резервы (5420, 5440, 5450, 5470)</t>
+  </si>
+  <si>
+    <t>Нераспределенная прибыль (непокрытый убыток) (5510, 5520)</t>
+  </si>
+  <si>
+    <t>Итого капитал (сумма строк 47-52)</t>
+  </si>
+  <si>
+    <t>Всего обязательства и капитал (сумма строк 37, 45, 53)</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
   </si>
 </sst>
 </file>
@@ -1416,22 +537,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="10"/>
+      <sz val="10"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="10"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="2"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -1487,7 +608,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1535,15 +656,11 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1593,11 +710,9 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1605,7 +720,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1927,10 +1047,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65:F65"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2720,8 +1840,8 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="46" t="s">
-        <v>126</v>
+      <c r="C2" s="43" t="s">
+        <v>80</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>4</v>
@@ -2750,29 +1870,29 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
       <c r="F7" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
+      <c r="A10" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -2823,8 +1943,8 @@
         <v>16</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
     </row>
@@ -2837,830 +1957,860 @@
         <v>18</v>
       </c>
       <c r="D16" s="17"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
       <c r="G16" s="14"/>
       <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>20</v>
-      </c>
       <c r="D17" s="17"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
       <c r="G17" s="19"/>
       <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="16" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D18" s="17"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
       <c r="G18" s="19"/>
       <c r="H18" s="18"/>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="16" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D19" s="17"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
       <c r="G19" s="19"/>
       <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="16" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D20" s="17"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
       <c r="G20" s="19"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="16" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D21" s="17"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
       <c r="G21" s="19"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="16" t="s">
-        <v>29</v>
+      <c r="B22" s="49" t="s">
+        <v>89</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D22" s="17"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
       <c r="G22" s="14"/>
       <c r="H22" s="18"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="16" t="s">
-        <v>31</v>
+      <c r="B23" s="49" t="s">
+        <v>90</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D23" s="17"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
       <c r="G23" s="19"/>
       <c r="H23" s="18"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
-      <c r="B24" s="16" t="s">
-        <v>33</v>
+      <c r="B24" s="49" t="s">
+        <v>91</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D24" s="17"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
       <c r="G24" s="19"/>
       <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
-      <c r="B25" s="16" t="s">
-        <v>35</v>
+      <c r="B25" s="49" t="s">
+        <v>92</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D25" s="17"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
       <c r="G25" s="19"/>
       <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
-      <c r="B26" s="16" t="s">
-        <v>37</v>
+      <c r="B26" s="49" t="s">
+        <v>93</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D26" s="17"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="44"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="42"/>
       <c r="G26" s="19"/>
       <c r="H26" s="18"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
-      <c r="B27" s="20" t="s">
-        <v>39</v>
+      <c r="B27" s="49" t="s">
+        <v>94</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
       <c r="G27" s="14"/>
       <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
-      <c r="B28" s="12" t="s">
-        <v>41</v>
+      <c r="B28" s="50" t="s">
+        <v>95</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="D28" s="12"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="22"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="21"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
-      <c r="B29" s="16" t="s">
-        <v>42</v>
+      <c r="B29" s="50" t="s">
+        <v>30</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D29" s="17"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19"/>
       <c r="H29" s="18"/>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
-      <c r="B30" s="16" t="s">
-        <v>44</v>
+      <c r="B30" s="49" t="s">
+        <v>96</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D30" s="17"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="22"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="21"/>
       <c r="H30" s="18"/>
-      <c r="I30" s="23"/>
-    </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I30" s="22"/>
+    </row>
+    <row r="31" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
-      <c r="B31" s="16" t="s">
-        <v>46</v>
+      <c r="B31" s="49" t="s">
+        <v>97</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D31" s="17"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="19"/>
       <c r="H31" s="18"/>
     </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
-      <c r="B32" s="16" t="s">
-        <v>48</v>
+      <c r="B32" s="49" t="s">
+        <v>98</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D32" s="17"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="19"/>
       <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
-      <c r="B33" s="16" t="s">
-        <v>50</v>
+      <c r="B33" s="49" t="s">
+        <v>99</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D33" s="17"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19"/>
       <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
-      <c r="B34" s="16" t="s">
-        <v>52</v>
+      <c r="B34" s="49" t="s">
+        <v>100</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D34" s="17"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19"/>
       <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
-      <c r="B35" s="16" t="s">
-        <v>54</v>
+      <c r="B35" s="49" t="s">
+        <v>101</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D35" s="17"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19"/>
       <c r="H35" s="18"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
-      <c r="B36" s="16" t="s">
-        <v>56</v>
+      <c r="B36" s="49" t="s">
+        <v>102</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D36" s="17"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19"/>
       <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="16" t="s">
-        <v>58</v>
+      <c r="B37" s="49" t="s">
+        <v>103</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="19"/>
       <c r="H37" s="18"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
-      <c r="B38" s="16" t="s">
-        <v>60</v>
+      <c r="B38" s="49" t="s">
+        <v>104</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="D38" s="17"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
       <c r="G38" s="14"/>
       <c r="H38" s="18"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
-      <c r="B39" s="24" t="s">
-        <v>62</v>
+      <c r="B39" s="49" t="s">
+        <v>105</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="D39" s="13"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="22"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="21"/>
       <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
-      <c r="B40" s="24" t="s">
-        <v>64</v>
+      <c r="B40" s="49" t="s">
+        <v>106</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D40" s="25"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="22"/>
+        <v>82</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="21"/>
       <c r="H40" s="18"/>
-      <c r="I40" s="23"/>
+      <c r="I40" s="22"/>
       <c r="J40" s="18"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
-      <c r="B41" s="12" t="s">
-        <v>65</v>
+      <c r="B41" s="50" t="s">
+        <v>107</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="D41" s="12"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
       <c r="G41" s="14"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
-      <c r="B42" s="16" t="s">
-        <v>66</v>
+      <c r="B42" s="50" t="s">
+        <v>108</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="D42" s="17"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
       <c r="G42" s="14"/>
     </row>
-    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
-      <c r="B43" s="16" t="s">
-        <v>68</v>
+      <c r="B43" s="50" t="s">
+        <v>42</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="D43" s="17"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="41"/>
       <c r="G43" s="19"/>
     </row>
-    <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
-      <c r="B44" s="16" t="s">
-        <v>70</v>
+      <c r="B44" s="49" t="s">
+        <v>109</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="D44" s="17"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
       <c r="G44" s="14"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
-      <c r="B45" s="16" t="s">
-        <v>72</v>
+      <c r="B45" s="49" t="s">
+        <v>110</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="D45" s="17"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
       <c r="G45" s="19"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
-      <c r="B46" s="16" t="s">
-        <v>74</v>
+      <c r="B46" s="49" t="s">
+        <v>111</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="D46" s="17"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
       <c r="G46" s="19"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
-      <c r="B47" s="16" t="s">
-        <v>76</v>
+      <c r="B47" s="49" t="s">
+        <v>112</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D47" s="17"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
       <c r="G47" s="19"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
-      <c r="B48" s="16" t="s">
-        <v>78</v>
+      <c r="B48" s="49" t="s">
+        <v>113</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D48" s="17"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
       <c r="G48" s="19"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
-      <c r="B49" s="24" t="s">
-        <v>80</v>
+      <c r="B49" s="49" t="s">
+        <v>114</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="D49" s="13"/>
-      <c r="E49" s="51"/>
-      <c r="F49" s="51"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
       <c r="G49" s="14"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
-      <c r="B50" s="12" t="s">
-        <v>82</v>
+      <c r="B50" s="49" t="s">
+        <v>115</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D50" s="17"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
       <c r="G50" s="19"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
-      <c r="B51" s="16" t="s">
-        <v>84</v>
+      <c r="B51" s="49" t="s">
+        <v>116</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="D51" s="17"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
       <c r="G51" s="19"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
-      <c r="B52" s="16" t="s">
-        <v>86</v>
+      <c r="B52" s="50" t="s">
+        <v>51</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="D52" s="17"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
       <c r="G52" s="19"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
-      <c r="B53" s="16" t="s">
-        <v>88</v>
+      <c r="B53" s="49" t="s">
+        <v>117</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="D53" s="17"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
       <c r="G53" s="19"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
-      <c r="B54" s="16" t="s">
-        <v>90</v>
+      <c r="B54" s="49" t="s">
+        <v>118</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="D54" s="17"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="43"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="41"/>
       <c r="G54" s="19"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
-      <c r="B55" s="16" t="s">
-        <v>92</v>
+      <c r="B55" s="49" t="s">
+        <v>119</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="D55" s="17"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="41"/>
       <c r="G55" s="19"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
-      <c r="B56" s="16" t="s">
-        <v>94</v>
+      <c r="B56" s="49" t="s">
+        <v>120</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="D56" s="17"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
       <c r="G56" s="19"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
-      <c r="B57" s="24" t="s">
-        <v>96</v>
+      <c r="B57" s="49" t="s">
+        <v>121</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="D57" s="13"/>
-      <c r="E57" s="47"/>
-      <c r="F57" s="47"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
       <c r="G57" s="19"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
-      <c r="B58" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C58" s="21">
+      <c r="B58" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="20">
         <v>44</v>
       </c>
       <c r="D58" s="12"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
       <c r="G58" s="19"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
-      <c r="B59" s="16" t="s">
-        <v>99</v>
+      <c r="B59" s="50" t="s">
+        <v>123</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="D59" s="17"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="43"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="41"/>
       <c r="G59" s="14"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
-      <c r="B60" s="45" t="s">
-        <v>123</v>
+      <c r="B60" s="50" t="s">
+        <v>60</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="D60" s="17"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="41"/>
       <c r="G60" s="19"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
-      <c r="B61" s="16" t="s">
-        <v>102</v>
+      <c r="B61" s="49" t="s">
+        <v>124</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="D61" s="17"/>
-      <c r="E61" s="43"/>
-      <c r="F61" s="43"/>
+      <c r="E61" s="41"/>
+      <c r="F61" s="41"/>
       <c r="G61" s="19"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
-      <c r="B62" s="16" t="s">
-        <v>104</v>
+      <c r="B62" s="49" t="s">
+        <v>125</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="D62" s="17"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="43"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="41"/>
       <c r="G62" s="19"/>
       <c r="H62" s="19"/>
       <c r="I62" s="19"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
-      <c r="B63" s="16" t="s">
-        <v>106</v>
+      <c r="B63" s="49" t="s">
+        <v>126</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="D63" s="17"/>
-      <c r="E63" s="42"/>
-      <c r="F63" s="42"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="40"/>
       <c r="G63" s="14"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
-      <c r="B64" s="16" t="s">
-        <v>108</v>
+      <c r="B64" s="49" t="s">
+        <v>127</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="D64" s="17"/>
-      <c r="E64" s="42"/>
-      <c r="F64" s="42"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
       <c r="G64" s="14"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
-      <c r="B65" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>111</v>
+      <c r="B65" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="D65" s="13"/>
-      <c r="E65" s="47"/>
-      <c r="F65" s="47"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="44"/>
       <c r="G65" s="19"/>
       <c r="H65" s="18"/>
-      <c r="I65" s="23"/>
+      <c r="I65" s="22"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
-      <c r="B66" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>113</v>
+      <c r="B66" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="D66" s="13"/>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47"/>
+      <c r="E66" s="44"/>
+      <c r="F66" s="44"/>
       <c r="G66" s="19"/>
-      <c r="I66" s="19"/>
-      <c r="J66" s="19"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="22"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="26"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
-      <c r="F67" s="29"/>
-      <c r="G67" s="23"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D67" s="13"/>
+      <c r="E67" s="44"/>
+      <c r="F67" s="44"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="22"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="26"/>
-      <c r="B68" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="C68" s="50"/>
-      <c r="D68" s="50"/>
-      <c r="E68" s="50"/>
-      <c r="F68" s="50"/>
+      <c r="A68" s="10"/>
+      <c r="B68" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D68" s="13"/>
+      <c r="E68" s="44"/>
+      <c r="F68" s="44"/>
       <c r="G68" s="19"/>
+      <c r="I68" s="19"/>
+      <c r="J68" s="19"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="26"/>
-      <c r="B69" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="C69" s="50"/>
-      <c r="D69" s="50"/>
-      <c r="E69" s="50"/>
-      <c r="F69" s="50"/>
+      <c r="A69" s="24"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="22"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="26"/>
-      <c r="B70" s="30"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="31"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="33"/>
-      <c r="G70" s="32"/>
+      <c r="A70" s="24"/>
+      <c r="B70" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C70" s="48"/>
+      <c r="D70" s="48"/>
+      <c r="E70" s="48"/>
+      <c r="F70" s="48"/>
+      <c r="G70" s="19"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E71" s="19"/>
+      <c r="A71" s="24"/>
+      <c r="B71" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C71" s="48"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="48"/>
+      <c r="F71" s="48"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B72" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F72" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="G72" s="35"/>
-      <c r="H72" s="19"/>
+      <c r="A72" s="24"/>
+      <c r="B72" s="28"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="30"/>
+      <c r="F72" s="31"/>
+      <c r="G72" s="30"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B73" s="34"/>
-      <c r="C73" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="D73" s="34"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="G73" s="35"/>
-      <c r="H73" s="19"/>
+      <c r="E73" s="19"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B74" s="34"/>
-      <c r="C74" s="34"/>
-      <c r="D74" s="34"/>
-      <c r="E74" s="34"/>
-      <c r="F74" s="34"/>
-      <c r="G74" s="35"/>
+      <c r="B74" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F74" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G74" s="33"/>
       <c r="H74" s="19"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B75" s="34"/>
-      <c r="F75" s="34"/>
-      <c r="G75" s="35"/>
+      <c r="B75" s="32"/>
+      <c r="C75" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D75" s="32"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="G75" s="33"/>
+      <c r="H75" s="19"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B76" s="38"/>
-      <c r="C76" s="34"/>
-      <c r="D76" s="34"/>
-      <c r="E76" s="35"/>
-      <c r="F76" s="37"/>
-      <c r="G76" s="35"/>
+      <c r="B76" s="32"/>
+      <c r="C76" s="32"/>
+      <c r="D76" s="32"/>
+      <c r="E76" s="32"/>
+      <c r="F76" s="32"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="19"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="39"/>
-      <c r="C77" s="34"/>
-      <c r="D77" s="34"/>
-      <c r="E77" s="34"/>
-      <c r="F77" s="34"/>
-      <c r="G77" s="35"/>
+      <c r="B77" s="32"/>
+      <c r="F77" s="32"/>
+      <c r="G77" s="33"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B78" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="C78" s="35"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="35"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="33"/>
       <c r="F78" s="35"/>
-      <c r="G78" s="35"/>
+      <c r="G78" s="33"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C79" s="35"/>
-      <c r="D79" s="35"/>
-      <c r="E79" s="35"/>
-      <c r="F79" s="35"/>
-      <c r="G79" s="35"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="32"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="33"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B80" s="39"/>
-      <c r="E80" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="F80" s="35"/>
-      <c r="G80" s="35"/>
+      <c r="B80" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C80" s="33"/>
+      <c r="D80" s="33"/>
+      <c r="E80" s="33"/>
+      <c r="F80" s="33"/>
+      <c r="G80" s="33"/>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B81" s="39"/>
-      <c r="C81" s="35"/>
-      <c r="D81" s="35"/>
-      <c r="E81" s="35"/>
-      <c r="F81" s="35"/>
-      <c r="G81" s="35"/>
+      <c r="C81" s="33"/>
+      <c r="D81" s="33"/>
+      <c r="E81" s="33"/>
+      <c r="F81" s="33"/>
+      <c r="G81" s="33"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="37"/>
+      <c r="E82" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="F82" s="33"/>
+      <c r="G82" s="33"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="37"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="33"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A10:F10"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.98425196850393704" right="0.59055118110236227" top="0.98425196850393704" bottom="0.98425196850393704" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>